<commit_message>
code studies commit 24/11/2020
</commit_message>
<xml_diff>
--- a/Python/PlayPython/Skool VS Koshuis/Input/Fees.xlsx
+++ b/Python/PlayPython/Skool VS Koshuis/Input/Fees.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymondk\Desktop\Study\Python\PlayPython\Skool VS Koshuis\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D22E1416-8892-4CA0-9FFE-3C399118A1C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E02A59F-DDF5-4FC8-B204-17D1806C0AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1">
-        <v>600</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -405,7 +405,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>1000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -416,7 +416,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>360</v>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>